<commit_message>
feat: add default sample
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Personal(Offline)\timetableGPT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6D910E-EA31-4553-921C-92BCD7A897D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54367559-88F7-4178-9EBC-077FA4B79D1A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11205" xr2:uid="{8FC4A9FE-E619-4128-9035-7F9E44AEF883}"/>
   </bookViews>
@@ -39,120 +39,6 @@
     <t>room</t>
   </si>
   <si>
-    <t>Room 251</t>
-  </si>
-  <si>
-    <t>Room 252</t>
-  </si>
-  <si>
-    <t>Room 253</t>
-  </si>
-  <si>
-    <t>Room 254</t>
-  </si>
-  <si>
-    <t>Room 255</t>
-  </si>
-  <si>
-    <t>Room 256</t>
-  </si>
-  <si>
-    <t>Room 261</t>
-  </si>
-  <si>
-    <t>Room 263</t>
-  </si>
-  <si>
-    <t>Room 266</t>
-  </si>
-  <si>
-    <t>Room 267</t>
-  </si>
-  <si>
-    <t>Room 321</t>
-  </si>
-  <si>
-    <t>Room 322</t>
-  </si>
-  <si>
-    <t>Room 323</t>
-  </si>
-  <si>
-    <t>Room 324</t>
-  </si>
-  <si>
-    <t>Room 326</t>
-  </si>
-  <si>
-    <t>Room 327</t>
-  </si>
-  <si>
-    <t>Room 328</t>
-  </si>
-  <si>
-    <t>Room 331</t>
-  </si>
-  <si>
-    <t>Room 332</t>
-  </si>
-  <si>
-    <t>Room 334</t>
-  </si>
-  <si>
-    <t>Room 335</t>
-  </si>
-  <si>
-    <t>Room 337</t>
-  </si>
-  <si>
-    <t>Room 341</t>
-  </si>
-  <si>
-    <t>Room 342</t>
-  </si>
-  <si>
-    <t>Room 343</t>
-  </si>
-  <si>
-    <t>Room 344</t>
-  </si>
-  <si>
-    <t>Room 345</t>
-  </si>
-  <si>
-    <t>Room 346</t>
-  </si>
-  <si>
-    <t>Room 347</t>
-  </si>
-  <si>
-    <t>Room 348</t>
-  </si>
-  <si>
-    <t>Room 257</t>
-  </si>
-  <si>
-    <t>Room 262</t>
-  </si>
-  <si>
-    <t>Room 264</t>
-  </si>
-  <si>
-    <t>Room 265</t>
-  </si>
-  <si>
-    <t>Room 325</t>
-  </si>
-  <si>
-    <t>Room 333</t>
-  </si>
-  <si>
-    <t>Room 338</t>
-  </si>
-  <si>
-    <t>Room 336</t>
-  </si>
-  <si>
     <t>Julian Gay</t>
   </si>
   <si>
@@ -319,6 +205,120 @@
   </si>
   <si>
     <t>Trinity Smith</t>
+  </si>
+  <si>
+    <t>R 251</t>
+  </si>
+  <si>
+    <t>R 252</t>
+  </si>
+  <si>
+    <t>R 253</t>
+  </si>
+  <si>
+    <t>R 254</t>
+  </si>
+  <si>
+    <t>R 255</t>
+  </si>
+  <si>
+    <t>R 256</t>
+  </si>
+  <si>
+    <t>R 261</t>
+  </si>
+  <si>
+    <t>R 263</t>
+  </si>
+  <si>
+    <t>R 266</t>
+  </si>
+  <si>
+    <t>R 267</t>
+  </si>
+  <si>
+    <t>R 321</t>
+  </si>
+  <si>
+    <t>R 322</t>
+  </si>
+  <si>
+    <t>R 323</t>
+  </si>
+  <si>
+    <t>R 324</t>
+  </si>
+  <si>
+    <t>R 326</t>
+  </si>
+  <si>
+    <t>R 327</t>
+  </si>
+  <si>
+    <t>R 328</t>
+  </si>
+  <si>
+    <t>R 331</t>
+  </si>
+  <si>
+    <t>R 332</t>
+  </si>
+  <si>
+    <t>R 334</t>
+  </si>
+  <si>
+    <t>R 335</t>
+  </si>
+  <si>
+    <t>R 337</t>
+  </si>
+  <si>
+    <t>R 341</t>
+  </si>
+  <si>
+    <t>R 342</t>
+  </si>
+  <si>
+    <t>R 343</t>
+  </si>
+  <si>
+    <t>R 344</t>
+  </si>
+  <si>
+    <t>R 345</t>
+  </si>
+  <si>
+    <t>R 346</t>
+  </si>
+  <si>
+    <t>R 347</t>
+  </si>
+  <si>
+    <t>R 348</t>
+  </si>
+  <si>
+    <t>R 257</t>
+  </si>
+  <si>
+    <t>R 262</t>
+  </si>
+  <si>
+    <t>R 264</t>
+  </si>
+  <si>
+    <t>R 265</t>
+  </si>
+  <si>
+    <t>R 325</t>
+  </si>
+  <si>
+    <t>R 333</t>
+  </si>
+  <si>
+    <t>R 338</t>
+  </si>
+  <si>
+    <t>R 336</t>
   </si>
 </sst>
 </file>
@@ -689,7 +689,7 @@
   <dimension ref="A1:D84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,7 +715,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2">
         <v>44963.5625</v>
@@ -724,12 +724,12 @@
         <v>44963.666666666664</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2">
         <v>44963.5625</v>
@@ -738,12 +738,12 @@
         <v>44963.631944444445</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2">
         <v>44963.5625</v>
@@ -752,12 +752,12 @@
         <v>44963.631944444445</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2">
         <v>44963.5625</v>
@@ -766,12 +766,12 @@
         <v>44963.631944444445</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2">
         <v>44963.5625</v>
@@ -780,12 +780,12 @@
         <v>44963.631944444445</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2">
         <v>44963.5625</v>
@@ -794,12 +794,12 @@
         <v>44963.631944444445</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>9</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2">
         <v>44963.5625</v>
@@ -808,12 +808,12 @@
         <v>44963.631944444445</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2">
         <v>44963.5625</v>
@@ -822,12 +822,12 @@
         <v>44963.631944444445</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2">
         <v>44963.5625</v>
@@ -836,12 +836,12 @@
         <v>44963.666666666664</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="B11" s="2">
         <v>44963.5625</v>
@@ -850,12 +850,12 @@
         <v>44963.631944444445</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="B12" s="2">
         <v>44963.5625</v>
@@ -864,12 +864,12 @@
         <v>44963.666666666664</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="B13" s="2">
         <v>44963.5625</v>
@@ -878,12 +878,12 @@
         <v>44963.666666666664</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="B14" s="2">
         <v>44963.5625</v>
@@ -892,12 +892,12 @@
         <v>44963.666666666664</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2">
         <v>44963.5625</v>
@@ -906,12 +906,12 @@
         <v>44963.666666666664</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="B16" s="2">
         <v>44963.5625</v>
@@ -920,12 +920,12 @@
         <v>44963.666666666664</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="B17" s="2">
         <v>44963.5625</v>
@@ -934,12 +934,12 @@
         <v>44963.666666666664</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="B18" s="2">
         <v>44963.5625</v>
@@ -948,12 +948,12 @@
         <v>44963.631944444445</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="B19" s="2">
         <v>44963.5625</v>
@@ -962,12 +962,12 @@
         <v>44963.666666666664</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="B20" s="2">
         <v>44963.5625</v>
@@ -976,12 +976,12 @@
         <v>44963.666666666664</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>61</v>
+        <v>23</v>
       </c>
       <c r="B21" s="2">
         <v>44963.5625</v>
@@ -990,12 +990,12 @@
         <v>44963.631944444445</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="B22" s="2">
         <v>44963.5625</v>
@@ -1004,12 +1004,12 @@
         <v>44963.666666666664</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>24</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="B23" s="2">
         <v>44963.5625</v>
@@ -1018,12 +1018,12 @@
         <v>44963.631944444445</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="B24" s="2">
         <v>44963.5625</v>
@@ -1032,12 +1032,12 @@
         <v>44963.631944444445</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>26</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>65</v>
+        <v>27</v>
       </c>
       <c r="B25" s="2">
         <v>44963.5625</v>
@@ -1046,12 +1046,12 @@
         <v>44963.631944444445</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="B26" s="2">
         <v>44963.5625</v>
@@ -1060,12 +1060,12 @@
         <v>44963.631944444445</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="B27" s="2">
         <v>44963.5625</v>
@@ -1074,12 +1074,12 @@
         <v>44963.666666666664</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>29</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="B28" s="2">
         <v>44963.5625</v>
@@ -1088,12 +1088,12 @@
         <v>44963.631944444445</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="B29" s="2">
         <v>44963.5625</v>
@@ -1102,12 +1102,12 @@
         <v>44963.666666666664</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="B30" s="2">
         <v>44963.5625</v>
@@ -1116,12 +1116,12 @@
         <v>44963.631944444445</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>32</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>71</v>
+        <v>33</v>
       </c>
       <c r="B31" s="2">
         <v>44963.5625</v>
@@ -1130,12 +1130,12 @@
         <v>44963.631944444445</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="B32" s="2">
         <v>44963.458333333336</v>
@@ -1144,12 +1144,12 @@
         <v>44963.527777777781</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="B33" s="2">
         <v>44963.458333333336</v>
@@ -1158,12 +1158,12 @@
         <v>44963.527777777781</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>8</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>73</v>
+        <v>35</v>
       </c>
       <c r="B34" s="2">
         <v>44963.458333333336</v>
@@ -1172,12 +1172,12 @@
         <v>44963.527777777781</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>9</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="B35" s="2">
         <v>44963.458333333336</v>
@@ -1186,12 +1186,12 @@
         <v>44963.527777777781</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="B36" s="2">
         <v>44963.458333333336</v>
@@ -1200,12 +1200,12 @@
         <v>44963.527777777781</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>35</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="B37" s="2">
         <v>44963.458333333336</v>
@@ -1214,12 +1214,12 @@
         <v>44963.527777777781</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="B38" s="2">
         <v>44963.458333333336</v>
@@ -1228,12 +1228,12 @@
         <v>44963.527777777781</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="B39" s="2">
         <v>44963.458333333336</v>
@@ -1242,12 +1242,12 @@
         <v>44963.527777777781</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="B40" s="2">
         <v>44963.458333333336</v>
@@ -1256,12 +1256,12 @@
         <v>44963.527777777781</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="B41" s="2">
         <v>44963.458333333336</v>
@@ -1270,12 +1270,12 @@
         <v>44963.527777777781</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="B42" s="2">
         <v>44963.458333333336</v>
@@ -1284,12 +1284,12 @@
         <v>44963.527777777781</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="B43" s="2">
         <v>44963.458333333336</v>
@@ -1298,12 +1298,12 @@
         <v>44963.527777777781</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="B44" s="2">
         <v>44963.458333333336</v>
@@ -1312,12 +1312,12 @@
         <v>44963.527777777781</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>26</v>
+        <v>82</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>71</v>
+        <v>33</v>
       </c>
       <c r="B45" s="2">
         <v>44963.458333333336</v>
@@ -1326,12 +1326,12 @@
         <v>44963.527777777781</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="B46" s="2">
         <v>44963.458333333336</v>
@@ -1340,12 +1340,12 @@
         <v>44963.527777777781</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="B47" s="2">
         <v>44963.458333333336</v>
@@ -1354,12 +1354,12 @@
         <v>44963.527777777781</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="B48" s="2">
         <v>44963.458333333336</v>
@@ -1368,12 +1368,12 @@
         <v>44963.527777777781</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>32</v>
+        <v>88</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
       <c r="B49" s="2">
         <v>44963.423611111109</v>
@@ -1382,12 +1382,12 @@
         <v>44963.527777777781</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="B50" s="2">
         <v>44963.423611111109</v>
@@ -1396,12 +1396,12 @@
         <v>44963.527777777781</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="B51" s="2">
         <v>44963.423611111109</v>
@@ -1410,12 +1410,12 @@
         <v>44963.527777777781</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>82</v>
+        <v>44</v>
       </c>
       <c r="B52" s="2">
         <v>44963.423611111109</v>
@@ -1424,12 +1424,12 @@
         <v>44963.527777777781</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="B53" s="2">
         <v>44963.423611111109</v>
@@ -1438,12 +1438,12 @@
         <v>44963.527777777781</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>39</v>
+        <v>95</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>83</v>
+        <v>45</v>
       </c>
       <c r="B54" s="2">
         <v>44963.423611111109</v>
@@ -1452,12 +1452,12 @@
         <v>44963.527777777781</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>84</v>
+        <v>46</v>
       </c>
       <c r="B55" s="2">
         <v>44963.423611111109</v>
@@ -1466,12 +1466,12 @@
         <v>44963.527777777781</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>24</v>
+        <v>80</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="B56" s="2">
         <v>44963.423611111109</v>
@@ -1480,12 +1480,12 @@
         <v>44963.527777777781</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>40</v>
+        <v>96</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="B57" s="2">
         <v>44963.423611111109</v>
@@ -1494,12 +1494,12 @@
         <v>44963.527777777781</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>29</v>
+        <v>85</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="B58" s="2">
         <v>44963.423611111109</v>
@@ -1508,12 +1508,12 @@
         <v>44963.527777777781</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="B59" s="2">
         <v>44963.423611111109</v>
@@ -1522,12 +1522,12 @@
         <v>44963.527777777781</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="B60" s="2">
         <v>44963.381944444445</v>
@@ -1536,12 +1536,12 @@
         <v>44963.451388888891</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="B61" s="2">
         <v>44963.381944444445</v>
@@ -1550,12 +1550,12 @@
         <v>44963.451388888891</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>8</v>
+        <v>64</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="B62" s="2">
         <v>44963.381944444445</v>
@@ -1564,12 +1564,12 @@
         <v>44963.451388888891</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>9</v>
+        <v>65</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="B63" s="2">
         <v>44963.381944444445</v>
@@ -1578,12 +1578,12 @@
         <v>44963.486111111109</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="B64" s="2">
         <v>44963.381944444445</v>
@@ -1592,12 +1592,12 @@
         <v>44963.451388888891</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>61</v>
+        <v>23</v>
       </c>
       <c r="B65" s="2">
         <v>44963.381944444445</v>
@@ -1606,12 +1606,12 @@
         <v>44963.451388888891</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>35</v>
+        <v>91</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>89</v>
+        <v>51</v>
       </c>
       <c r="B66" s="2">
         <v>44963.381944444445</v>
@@ -1620,12 +1620,12 @@
         <v>44963.486111111109</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>65</v>
+        <v>27</v>
       </c>
       <c r="B67" s="2">
         <v>44963.381944444445</v>
@@ -1634,12 +1634,12 @@
         <v>44963.451388888891</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="B68" s="2">
         <v>44963.381944444445</v>
@@ -1648,12 +1648,12 @@
         <v>44963.451388888891</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>91</v>
+        <v>53</v>
       </c>
       <c r="B69" s="2">
         <v>44963.381944444445</v>
@@ -1662,12 +1662,12 @@
         <v>44963.486111111109</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="B70" s="2">
         <v>44963.381944444445</v>
@@ -1676,12 +1676,12 @@
         <v>44963.451388888891</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>92</v>
+        <v>54</v>
       </c>
       <c r="B71" s="2">
         <v>44963.381944444445</v>
@@ -1690,12 +1690,12 @@
         <v>44963.451388888891</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>93</v>
+        <v>55</v>
       </c>
       <c r="B72" s="2">
         <v>44963.381944444445</v>
@@ -1704,12 +1704,12 @@
         <v>44963.486111111109</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="B73" s="2">
         <v>44963.381944444445</v>
@@ -1718,12 +1718,12 @@
         <v>44963.451388888891</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>94</v>
+        <v>56</v>
       </c>
       <c r="B74" s="2">
         <v>44963.381944444445</v>
@@ -1732,12 +1732,12 @@
         <v>44963.486111111109</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="B75" s="2">
         <v>44963.381944444445</v>
@@ -1746,12 +1746,12 @@
         <v>44963.451388888891</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="B76" s="2">
         <v>44963.381944444445</v>
@@ -1760,12 +1760,12 @@
         <v>44963.451388888891</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="B77" s="2">
         <v>44963.381944444445</v>
@@ -1774,12 +1774,12 @@
         <v>44963.451388888891</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="B78" s="2">
         <v>44963.381944444445</v>
@@ -1788,12 +1788,12 @@
         <v>44963.451388888891</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="B79" s="2">
         <v>44963.381944444445</v>
@@ -1802,12 +1802,12 @@
         <v>44963.451388888891</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>32</v>
+        <v>88</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
       <c r="B80" s="2">
         <v>44963.305555555555</v>
@@ -1816,12 +1816,12 @@
         <v>44963.409722222219</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>95</v>
+        <v>57</v>
       </c>
       <c r="B81" s="2">
         <v>44963.305555555555</v>
@@ -1830,12 +1830,12 @@
         <v>44963.375</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>96</v>
+        <v>58</v>
       </c>
       <c r="B82" s="2">
         <v>44963.305555555555</v>
@@ -1844,12 +1844,12 @@
         <v>44963.375</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="B83" s="2">
         <v>44963.305555555555</v>
@@ -1858,12 +1858,12 @@
         <v>44963.409722222219</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>97</v>
+        <v>59</v>
       </c>
       <c r="B84" s="2">
         <v>44963.305555555555</v>
@@ -1872,7 +1872,7 @@
         <v>44963.375</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>29</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>